<commit_message>
workflowr::wflow_publish(c("./docs/*", "./analysis/*", "./code/*",     "./output/*"))
</commit_message>
<xml_diff>
--- a/docs/Descriptives.xlsx
+++ b/docs/Descriptives.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -354,45 +354,40 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T/NK   N=22</t>
+          <t>Microglia_1   N=476</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Microglia_0   N=186</t>
+          <t>Microglia_2   N=160</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Microglia_1   N=164</t>
+          <t>Microglia_3   N=143</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Microglia_2   N=107</t>
+          <t>Microglia_4   N=45</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Microglia_3   N=99</t>
+          <t>Granulocytes   N=27</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Microglia_4   N=26</t>
+          <t>Microglia_5   N=19</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Microglia_5   N=23</t>
+          <t>Mono/Mac   N=35</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Granulocytes   N=22</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>p.overall</t>
         </is>
@@ -406,17 +401,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -431,7 +426,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -440,11 +435,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t xml:space="preserve">    .    </t>
         </is>
@@ -458,45 +448,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
+          <t xml:space="preserve">  91 (19.1%)   </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  27 (14.5%)  </t>
+          <t xml:space="preserve">  40 (25.0%)   </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (12.8%)  </t>
+          <t xml:space="preserve">  52 (36.4%)   </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (10.3%)  </t>
+          <t xml:space="preserve">  8 (17.8%)   </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (11.1%)  </t>
+          <t xml:space="preserve">  13 (48.1%)  </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (3.85%)   </t>
+          <t xml:space="preserve">   5 (26.3%)   </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 (8.70%)   </t>
+          <t xml:space="preserve">  8 (22.9%)   </t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  8 (36.4%)   </t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -510,45 +495,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  16 (72.7%)  </t>
+          <t xml:space="preserve">  385 (80.9%)  </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 159 (85.5%)  </t>
+          <t xml:space="preserve">  120 (75.0%)  </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 143 (87.2%)  </t>
+          <t xml:space="preserve">  91 (63.6%)   </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  96 (89.7%)  </t>
+          <t xml:space="preserve">  37 (82.2%)  </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  88 (88.9%)  </t>
+          <t xml:space="preserve">  14 (51.9%)  </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  25 (96.2%)  </t>
+          <t xml:space="preserve">  14 (73.7%)   </t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (91.3%)  </t>
+          <t xml:space="preserve">  27 (77.1%)  </t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  14 (63.6%)  </t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -562,17 +542,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -587,7 +567,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -597,62 +577,52 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &lt;0.001  </t>
+          <t xml:space="preserve">    .    </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    10</t>
+          <t xml:space="preserve">    37 weeks</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  13 (59.1%)  </t>
+          <t xml:space="preserve">  295 (62.0%)  </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  65 (34.9%)  </t>
+          <t xml:space="preserve">  100 (62.5%)  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  35 (21.3%)  </t>
+          <t xml:space="preserve">  83 (58.0%)   </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  26 (24.3%)  </t>
+          <t xml:space="preserve">  14 (31.1%)  </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  32 (32.3%)  </t>
+          <t xml:space="preserve">  15 (55.6%)  </t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (23.1%)   </t>
+          <t xml:space="preserve">   8 (42.1%)   </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  12 (52.2%)  </t>
+          <t xml:space="preserve">  18 (51.4%)  </t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  9 (40.9%)   </t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -661,50 +631,45 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    17</t>
+          <t xml:space="preserve">    38 weeks</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  49 (10.3%)   </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  19 (10.2%)  </t>
+          <t xml:space="preserve">  11 (6.88%)   </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  68 (41.5%)  </t>
+          <t xml:space="preserve">  16 (11.2%)   </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 (29.0%)  </t>
+          <t xml:space="preserve">  3 (6.67%)   </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  29 (29.3%)  </t>
+          <t xml:space="preserve">  3 (11.1%)   </t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (42.3%)  </t>
+          <t xml:space="preserve">   4 (21.1%)   </t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.0%)   </t>
+          <t xml:space="preserve">  4 (11.4%)   </t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -713,50 +678,45 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">    9</t>
+          <t xml:space="preserve">    40 weeks</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8 (36.4%)   </t>
+          <t xml:space="preserve">  132 (27.7%)  </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 102 (54.8%)  </t>
+          <t xml:space="preserve">  49 (30.6%)   </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  61 (37.2%)  </t>
+          <t xml:space="preserve">  44 (30.8%)   </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  50 (46.7%)  </t>
+          <t xml:space="preserve">  28 (62.2%)  </t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  38 (38.4%)  </t>
+          <t xml:space="preserve">  9 (33.3%)   </t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9 (34.6%)   </t>
+          <t xml:space="preserve">   7 (36.8%)   </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8 (34.8%)   </t>
+          <t xml:space="preserve">  13 (37.1%)  </t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  13 (59.1%)  </t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -770,17 +730,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -795,7 +755,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -805,12 +765,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &lt;0.001  </t>
+          <t xml:space="preserve">  0.506  </t>
         </is>
       </c>
     </row>
@@ -822,45 +777,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.6%)   </t>
+          <t xml:space="preserve">  200 (42.0%)  </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  66 (35.5%)  </t>
+          <t xml:space="preserve">  65 (40.6%)   </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  93 (56.7%)  </t>
+          <t xml:space="preserve">  61 (42.7%)   </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  51 (47.7%)  </t>
+          <t xml:space="preserve">  14 (31.1%)  </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  44 (44.4%)  </t>
+          <t xml:space="preserve">  9 (33.3%)   </t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  15 (57.7%)  </t>
+          <t xml:space="preserve">  10 (52.6%)   </t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (47.8%)  </t>
+          <t xml:space="preserve">  18 (51.4%)  </t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -874,45 +824,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  19 (86.4%)  </t>
+          <t xml:space="preserve">  276 (58.0%)  </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 120 (64.5%)  </t>
+          <t xml:space="preserve">  95 (59.4%)   </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  71 (43.3%)  </t>
+          <t xml:space="preserve">  82 (57.3%)   </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  56 (52.3%)  </t>
+          <t xml:space="preserve">  31 (68.9%)  </t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  55 (55.6%)  </t>
+          <t xml:space="preserve">  18 (66.7%)  </t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (42.3%)  </t>
+          <t xml:space="preserve">   9 (47.4%)   </t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  12 (52.2%)  </t>
+          <t xml:space="preserve">  17 (48.6%)  </t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  16 (72.7%)  </t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -926,17 +871,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -951,7 +896,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -960,11 +905,6 @@
         </is>
       </c>
       <c r="I12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
         <is>
           <t xml:space="preserve"> &lt;0.001  </t>
         </is>
@@ -978,45 +918,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.6%)   </t>
+          <t xml:space="preserve">  337 (70.8%)  </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 101 (54.3%)  </t>
+          <t xml:space="preserve">  96 (60.0%)   </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 113 (68.9%)  </t>
+          <t xml:space="preserve">  70 (49.0%)   </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  70 (65.4%)  </t>
+          <t xml:space="preserve">  13 (28.9%)  </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  68 (68.7%)  </t>
+          <t xml:space="preserve">  5 (18.5%)   </t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (80.8%)  </t>
+          <t xml:space="preserve">  13 (68.4%)   </t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  12 (52.2%)  </t>
+          <t xml:space="preserve">  13 (37.1%)  </t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1030,45 +965,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  19 (86.4%)  </t>
+          <t xml:space="preserve">  139 (29.2%)  </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  85 (45.7%)  </t>
+          <t xml:space="preserve">  64 (40.0%)   </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  51 (31.1%)  </t>
+          <t xml:space="preserve">  73 (51.0%)   </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  37 (34.6%)  </t>
+          <t xml:space="preserve">  32 (71.1%)  </t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 (31.3%)  </t>
+          <t xml:space="preserve">  22 (81.5%)  </t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (19.2%)   </t>
+          <t xml:space="preserve">   6 (31.6%)   </t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (47.8%)  </t>
+          <t xml:space="preserve">  22 (62.9%)  </t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  20 (90.9%)  </t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1082,17 +1012,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1107,7 +1037,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1116,11 +1046,6 @@
         </is>
       </c>
       <c r="I15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
         <is>
           <t xml:space="preserve">    .    </t>
         </is>
@@ -1134,45 +1059,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
+          <t xml:space="preserve">  220 (46.2%)  </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  82 (44.1%)  </t>
+          <t xml:space="preserve">  54 (33.8%)   </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  45 (27.4%)  </t>
+          <t xml:space="preserve">  21 (14.7%)   </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  39 (36.4%)  </t>
+          <t xml:space="preserve">  3 (6.67%)   </t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  39 (39.4%)  </t>
+          <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  10 (38.5%)  </t>
+          <t xml:space="preserve">   8 (42.1%)   </t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9 (39.1%)   </t>
+          <t xml:space="preserve">  5 (14.3%)   </t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1186,45 +1106,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  17 (77.3%)  </t>
+          <t xml:space="preserve">  56 (11.8%)   </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  38 (20.4%)  </t>
+          <t xml:space="preserve">  41 (25.6%)   </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  26 (15.9%)  </t>
+          <t xml:space="preserve">  61 (42.7%)   </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  17 (15.9%)  </t>
+          <t xml:space="preserve">  28 (62.2%)  </t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  16 (16.2%)  </t>
+          <t xml:space="preserve">  18 (66.7%)  </t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (3.85%)   </t>
+          <t xml:space="preserve">   1 (5.26%)   </t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.0%)   </t>
+          <t xml:space="preserve">  12 (34.3%)  </t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  14 (63.6%)  </t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1238,45 +1153,40 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  117 (24.6%)  </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  19 (10.2%)  </t>
+          <t xml:space="preserve">  42 (26.2%)   </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  68 (41.5%)  </t>
+          <t xml:space="preserve">  49 (34.3%)   </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 (29.0%)  </t>
+          <t xml:space="preserve">  10 (22.2%)  </t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  29 (29.3%)  </t>
+          <t xml:space="preserve">  5 (18.5%)   </t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (42.3%)  </t>
+          <t xml:space="preserve">   5 (26.3%)   </t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.0%)   </t>
+          <t xml:space="preserve">  8 (22.9%)   </t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1290,45 +1200,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
+          <t xml:space="preserve">  83 (17.4%)   </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  47 (25.3%)  </t>
+          <t xml:space="preserve">  23 (14.4%)   </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  25 (15.2%)  </t>
+          <t xml:space="preserve">  12 (8.39%)   </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  20 (18.7%)  </t>
+          <t xml:space="preserve">  4 (8.89%)   </t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  15 (15.2%)  </t>
+          <t xml:space="preserve">  4 (14.8%)   </t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4 (15.4%)   </t>
+          <t xml:space="preserve">   5 (26.3%)   </t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8 (34.8%)   </t>
+          <t xml:space="preserve">  10 (28.6%)  </t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1342,17 +1247,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1367,7 +1272,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1377,12 +1282,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0.002  </t>
+          <t xml:space="preserve">    .    </t>
         </is>
       </c>
     </row>
@@ -1394,45 +1294,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  211 (44.3%)  </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  79 (42.5%)  </t>
+          <t xml:space="preserve">  60 (37.5%)   </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  70 (42.7%)  </t>
+          <t xml:space="preserve">  46 (32.2%)   </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  59 (55.1%)  </t>
+          <t xml:space="preserve">  20 (44.4%)  </t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  42 (42.4%)  </t>
+          <t xml:space="preserve">  8 (29.6%)   </t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  12 (46.2%)  </t>
+          <t xml:space="preserve">  12 (63.2%)   </t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  14 (60.9%)  </t>
+          <t xml:space="preserve">  12 (34.3%)  </t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  5 (22.7%)   </t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1446,45 +1341,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (50.0%)  </t>
+          <t xml:space="preserve">  114 (23.9%)  </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  50 (26.9%)  </t>
+          <t xml:space="preserve">  38 (23.8%)   </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  38 (23.2%)  </t>
+          <t xml:space="preserve">  40 (28.0%)   </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  17 (15.9%)  </t>
+          <t xml:space="preserve">  11 (24.4%)  </t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (21.2%)  </t>
+          <t xml:space="preserve">  11 (40.7%)  </t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (23.1%)   </t>
+          <t xml:space="preserve">   3 (15.8%)   </t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4 (17.4%)   </t>
+          <t xml:space="preserve">  13 (37.1%)  </t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  11 (50.0%)  </t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1498,45 +1388,40 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  10 (45.5%)  </t>
+          <t xml:space="preserve">  151 (31.7%)  </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  57 (30.6%)  </t>
+          <t xml:space="preserve">  62 (38.8%)   </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  56 (34.1%)  </t>
+          <t xml:space="preserve">  57 (39.9%)   </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 (29.0%)  </t>
+          <t xml:space="preserve">  14 (31.1%)  </t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  36 (36.4%)  </t>
+          <t xml:space="preserve">  8 (29.6%)   </t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8 (30.8%)   </t>
+          <t xml:space="preserve">   4 (21.1%)   </t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (21.7%)   </t>
+          <t xml:space="preserve">  10 (28.6%)  </t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1550,47 +1435,42 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t xml:space="preserve">  3.65 (1.91)  </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  8.25 (1.04)  </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  11.4 (1.55)  </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t xml:space="preserve">    . (.)     </t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 12.9 (1.50)  </t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 4.23 (1.73)  </t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8.66 (2.14)  </t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.17 (1.76)  </t>
+          <t xml:space="preserve"> 25.4 (0.15)  </t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
+          <t xml:space="preserve">  0.37 (0.28)  </t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
           <t xml:space="preserve">    . (.)     </t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 16.9 (0.61)  </t>
-        </is>
-      </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t xml:space="preserve">    . (.)     </t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> &lt;0.001  </t>
+          <t xml:space="preserve">  0.000  </t>
         </is>
       </c>
     </row>
@@ -1602,17 +1482,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1627,7 +1507,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1636,11 +1516,6 @@
         </is>
       </c>
       <c r="I25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
         <is>
           <t xml:space="preserve"> &lt;0.001  </t>
         </is>
@@ -1654,45 +1529,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.6%)   </t>
+          <t xml:space="preserve">  337 (70.8%)  </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 101 (54.3%)  </t>
+          <t xml:space="preserve">  96 (60.0%)   </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 113 (68.9%)  </t>
+          <t xml:space="preserve">  70 (49.0%)   </t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  70 (65.4%)  </t>
+          <t xml:space="preserve">  13 (28.9%)  </t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  68 (68.7%)  </t>
+          <t xml:space="preserve">  5 (18.5%)   </t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (80.8%)  </t>
+          <t xml:space="preserve">  13 (68.4%)   </t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  12 (52.2%)  </t>
+          <t xml:space="preserve">  13 (37.1%)  </t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1706,45 +1576,40 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  19 (86.4%)  </t>
+          <t xml:space="preserve">  139 (29.2%)  </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  85 (45.7%)  </t>
+          <t xml:space="preserve">  64 (40.0%)   </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  51 (31.1%)  </t>
+          <t xml:space="preserve">  73 (51.0%)   </t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  37 (34.6%)  </t>
+          <t xml:space="preserve">  32 (71.1%)  </t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 (31.3%)  </t>
+          <t xml:space="preserve">  22 (81.5%)  </t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (19.2%)   </t>
+          <t xml:space="preserve">   6 (31.6%)   </t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (47.8%)  </t>
+          <t xml:space="preserve">  22 (62.9%)  </t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  20 (90.9%)  </t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -1758,47 +1623,42 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>164049 (80916)</t>
+          <t xml:space="preserve">144231 (99988) </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>150451 (78955)</t>
+          <t>165293 (106792)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>134224 (54802)</t>
+          <t>101350 (115577)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>170420 (76702)</t>
+          <t>45112 (115701)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>152640 (72678)</t>
+          <t>128528 (83221)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>172200 (70772)</t>
+          <t>156629 (113020)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>176087 (64299)</t>
+          <t>139846 (82161)</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>144828 (65899)</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0.002  </t>
+          <t xml:space="preserve"> &lt;0.001  </t>
         </is>
       </c>
     </row>
@@ -1810,97 +1670,87 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>165078 (81748)</t>
+          <t>144728 (100322)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>150942 (78850)</t>
+          <t>165698 (106875)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>134355 (54810)</t>
+          <t>102184 (115632)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>170750 (76639)</t>
+          <t>45218 (115828)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>152790 (72668)</t>
+          <t>128986 (83445)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>172433 (70717)</t>
+          <t>157045 (113080)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>176390 (64225)</t>
+          <t>140931 (82079)</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>145316 (65972)</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0.002  </t>
+          <t xml:space="preserve"> &lt;0.001  </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>percent.mito</t>
+          <t>percent.mt</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.23 (0.90)  </t>
+          <t xml:space="preserve">  1.84 (1.32)  </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.75 (1.17)  </t>
+          <t xml:space="preserve">  2.44 (1.89)  </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.62 (1.01)  </t>
+          <t xml:space="preserve">  1.37 (1.37)  </t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.07 (1.07)  </t>
+          <t xml:space="preserve"> 1.05 (1.56)  </t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.72 (1.15)  </t>
+          <t xml:space="preserve"> 0.86 (0.96)  </t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1.97 (1.02)  </t>
+          <t xml:space="preserve">  1.98 (0.91)  </t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.11 (0.77)  </t>
+          <t xml:space="preserve"> 1.99 (1.37)  </t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.92 (1.00)  </t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
         <is>
           <t xml:space="preserve"> &lt;0.001  </t>
         </is>
@@ -1909,50 +1759,45 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>percent.ribo</t>
+          <t>percent.rp</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 6.53 (2.72)  </t>
+          <t xml:space="preserve">  2.10 (1.25)  </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.68 (1.58)  </t>
+          <t xml:space="preserve">  2.82 (2.11)  </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.75 (1.81)  </t>
+          <t xml:space="preserve">  1.10 (1.37)  </t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.44 (1.24)  </t>
+          <t xml:space="preserve"> 0.52 (0.67)  </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 3.28 (1.67)  </t>
+          <t xml:space="preserve"> 1.63 (0.96)  </t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.11 (0.85)  </t>
+          <t xml:space="preserve">  2.12 (1.25)  </t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.91 (1.35)  </t>
+          <t xml:space="preserve"> 3.14 (2.50)  </t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2.01 (1.17)  </t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
         <is>
           <t xml:space="preserve"> &lt;0.001  </t>
         </is>
@@ -1966,17 +1811,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1991,7 +1836,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t xml:space="preserve">              </t>
+          <t xml:space="preserve">               </t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2000,11 +1845,6 @@
         </is>
       </c>
       <c r="I32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              </t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
         <is>
           <t xml:space="preserve">    .    </t>
         </is>
@@ -2013,50 +1853,45 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    23#15773</t>
+          <t xml:space="preserve">    256#1022</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t xml:space="preserve">  35 (7.35%)   </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  15 (9.38%)   </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  15 (10.5%)   </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3 (6.67%)   </t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
           <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  7 (3.76%)   </t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  25 (15.2%)  </t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  12 (11.2%)  </t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  17 (17.2%)  </t>
-        </is>
-      </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4 (15.4%)   </t>
+          <t xml:space="preserve">   1 (5.26%)   </t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.35%)   </t>
+          <t xml:space="preserve">  2 (5.71%)   </t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2065,50 +1900,45 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">    23#15774</t>
+          <t xml:space="preserve">    256#1023</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
+          <t xml:space="preserve">  33 (6.93%)   </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (0.54%)   </t>
+          <t xml:space="preserve">  16 (10.0%)   </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  30 (18.3%)  </t>
+          <t xml:space="preserve">  18 (12.6%)   </t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  10 (9.35%)  </t>
+          <t xml:space="preserve">  4 (8.89%)   </t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (6.06%)   </t>
+          <t xml:space="preserve">  2 (7.41%)   </t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (3.85%)   </t>
+          <t xml:space="preserve">   0 (0.00%)   </t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.35%)   </t>
+          <t xml:space="preserve">  2 (5.71%)   </t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2117,50 +1947,45 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    23#15792</t>
+          <t xml:space="preserve">    364#469</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  49 (10.3%)   </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (5.91%)  </t>
+          <t xml:space="preserve">  11 (6.88%)   </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  13 (7.93%)  </t>
+          <t xml:space="preserve">  16 (11.2%)   </t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9 (8.41%)   </t>
+          <t xml:space="preserve">  3 (6.67%)   </t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (6.06%)   </t>
+          <t xml:space="preserve">  3 (11.1%)   </t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (23.1%)   </t>
+          <t xml:space="preserve">   4 (21.1%)   </t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.35%)   </t>
+          <t xml:space="preserve">  4 (11.4%)   </t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2174,45 +1999,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  21 (4.41%)   </t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  14 (7.53%)  </t>
+          <t xml:space="preserve">   6 (3.75%)   </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9 (5.49%)   </t>
+          <t xml:space="preserve">  11 (7.69%)   </t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 (1.87%)   </t>
+          <t xml:space="preserve">  4 (8.89%)   </t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (6.06%)   </t>
+          <t xml:space="preserve">  1 (3.70%)   </t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (3.85%)   </t>
+          <t xml:space="preserve">   1 (5.26%)   </t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (21.7%)   </t>
+          <t xml:space="preserve">  6 (17.1%)   </t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  3 (13.6%)   </t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2226,45 +2046,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (50.0%)  </t>
+          <t xml:space="preserve">  14 (2.94%)   </t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  10 (5.38%)  </t>
+          <t xml:space="preserve">  12 (7.50%)   </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (3.05%)   </t>
+          <t xml:space="preserve">  25 (17.5%)   </t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (5.61%)   </t>
+          <t xml:space="preserve">  23 (51.1%)  </t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (5.05%)   </t>
+          <t xml:space="preserve">  8 (29.6%)   </t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
+          <t xml:space="preserve">   0 (0.00%)   </t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.35%)   </t>
+          <t xml:space="preserve">  7 (20.0%)   </t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2278,45 +2093,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  97 (20.4%)   </t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  41 (22.0%)  </t>
+          <t xml:space="preserve">  31 (19.4%)   </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (12.8%)  </t>
+          <t xml:space="preserve">   8 (5.59%)   </t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  18 (16.8%)  </t>
+          <t xml:space="preserve">  1 (2.22%)   </t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (21.2%)  </t>
+          <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (19.2%)   </t>
+          <t xml:space="preserve">   6 (31.6%)   </t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (26.1%)   </t>
+          <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  0 (0.00%)   </t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2330,45 +2140,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  62 (13.0%)   </t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  33 (17.7%)  </t>
+          <t xml:space="preserve">  17 (10.6%)   </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  16 (9.76%)  </t>
+          <t xml:space="preserve">   1 (0.70%)   </t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  18 (16.8%)  </t>
+          <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  9 (9.09%)   </t>
+          <t xml:space="preserve">  3 (11.1%)   </t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (11.5%)   </t>
+          <t xml:space="preserve">   4 (21.1%)   </t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.0%)   </t>
+          <t xml:space="preserve">  4 (11.4%)   </t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  3 (13.6%)   </t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2382,45 +2187,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (4.55%)   </t>
+          <t xml:space="preserve">  123 (25.8%)  </t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  41 (22.0%)  </t>
+          <t xml:space="preserve">  23 (14.4%)   </t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  24 (14.6%)  </t>
+          <t xml:space="preserve">  13 (9.09%)   </t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (19.6%)  </t>
+          <t xml:space="preserve">  2 (4.44%)   </t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  18 (18.2%)  </t>
+          <t xml:space="preserve">  0 (0.00%)   </t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 (19.2%)   </t>
+          <t xml:space="preserve">   2 (10.5%)   </t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 (13.0%)   </t>
+          <t xml:space="preserve">  5 (14.3%)   </t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  2 (9.09%)   </t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>
@@ -2434,45 +2234,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  6 (27.3%)   </t>
+          <t xml:space="preserve">  42 (8.82%)   </t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  28 (15.1%)  </t>
+          <t xml:space="preserve">  29 (18.1%)   </t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  21 (12.8%)  </t>
+          <t xml:space="preserve">  36 (25.2%)   </t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (10.3%)  </t>
+          <t xml:space="preserve">  5 (11.1%)   </t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  11 (11.1%)  </t>
+          <t xml:space="preserve">  10 (37.0%)  </t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 (3.85%)   </t>
+          <t xml:space="preserve">   1 (5.26%)   </t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 (8.70%)   </t>
+          <t xml:space="preserve">  5 (14.3%)   </t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  8 (36.4%)   </t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
         <is>
           <t xml:space="preserve">         </t>
         </is>

</xml_diff>